<commit_message>
changed dico, to verif
</commit_message>
<xml_diff>
--- a/BDD/Dictionnaire_SAE.xlsx
+++ b/BDD/Dictionnaire_SAE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Compte" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,17 +21,18 @@
     <sheet name="Tarif" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Prestation" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="Activité" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Horaire" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Spectacle" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Visite" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="Parc attraction" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="Restauration" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="Avis" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="Adresse" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="Tag" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="Image" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="Parametres" sheetId="23" state="hidden" r:id="rId24"/>
-    <sheet name="Grille tarifaire" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="Spectacle" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Visite" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Parc attraction" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Restauration" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Horaire" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="Adresse" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="Tag" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="Repas" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="Avis" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="Image" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="Parametres" sheetId="24" state="hidden" r:id="rId25"/>
+    <sheet name="Grille tarifaire" sheetId="25" state="visible" r:id="rId26"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="221">
   <si>
     <t xml:space="preserve">Dictionnaire des Données</t>
   </si>
@@ -343,7 +344,7 @@
     <t xml:space="preserve">{1..3}$</t>
   </si>
   <si>
-    <t xml:space="preserve">Tag d'une offre : cf. Tag</t>
+    <t xml:space="preserve">Tags d'une offre : cf. Tag</t>
   </si>
   <si>
     <t xml:space="preserve">Avis d'une offre : cf </t>
@@ -355,6 +356,9 @@
     <t xml:space="preserve">Prestations d’une Offre : cf Prestation</t>
   </si>
   <si>
+    <t xml:space="preserve">Images d’une Offres : cf Image</t>
+  </si>
+  <si>
     <t xml:space="preserve">Les Offres Générales qui ne sont pas dans la table Offre Payante</t>
   </si>
   <si>
@@ -418,6 +422,12 @@
     <t xml:space="preserve">durée de l'activité en heure</t>
   </si>
   <si>
+    <t xml:space="preserve">interval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{YYYY-MM-DD-HH-mm-ss}</t>
+  </si>
+  <si>
     <t xml:space="preserve">ageRequisA</t>
   </si>
   <si>
@@ -430,6 +440,105 @@
     <t xml:space="preserve">renseignement des prestations incluses dans le prix, héritée de Prestation</t>
   </si>
   <si>
+    <t xml:space="preserve">lié à une offre Générale par une relation 0..1---0..1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette relation a une contrainte XOR par rapport à Spectacle, Visite, Parc Attraction, Restaurant pour éviter qu’une offre soit liée à plusieurs catégorie d’offre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idSpectacle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identifiant du spectacle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capaciteS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre de personne pouvant participer au spectacle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dureeS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">durée du spectacle en minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idVisite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identifiant de la visite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dureeV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">durée de la visite en heure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visiteGuidee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">savoir si c'est une visite guidée ou non</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{true/false}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">langueV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si c'est une visite guidée, savoir en quelles langues elles sont disponibles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idParc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identifiant du parc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nbAttractions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre d'attraction du parc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">planParc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plan du parc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bytea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utiliser une url </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ageRequisP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age requis pour accéder aux attractions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">planParc (cf. image)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idRestauration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identifiant du code restauration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gammeDePrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gamme de prix de l'établissement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repasServi : cf. Repas</t>
+  </si>
+  <si>
     <t xml:space="preserve">idHoraire</t>
   </si>
   <si>
@@ -445,7 +554,7 @@
     <t xml:space="preserve">time</t>
   </si>
   <si>
-    <t xml:space="preserve">{0-9}{A-Za-z}:{0-9}{A-Za-z}</t>
+    <t xml:space="preserve">{JJ-HH-mm-ss}</t>
   </si>
   <si>
     <t xml:space="preserve">fermeture</t>
@@ -454,109 +563,43 @@
     <t xml:space="preserve">fermeture de l'activité</t>
   </si>
   <si>
-    <t xml:space="preserve">pauseDebut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pause du début généralement du midi de l'activité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pauseFin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pause de fin généralement du midi de l'activité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idSpectacle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">identifiant du spectacle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">capaciteS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">capacité d'acceuil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dureeS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">durée du spectacle en minutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idVisite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">identifiant de la visite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dureeV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">durée de la visite en heure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">visiteGuidee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">savoir si c'est une visite guidée ou non</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"visite guidé"(1) / "visite non-guidée"(0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">langueV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">si c'est une visite guidée, savoir en quelles langues elles sont disponibles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idParc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">identifiant du parc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nbAttractions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nombre d'attraction du parc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">planParc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plan du parc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bytea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">utiliser une url </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ageRequisP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age requis pour accéder aux attractions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">planParc (cf. image)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idRestauration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">identifiant du code restauration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gammeDePrix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gamme de prix de l'établissement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">repasServi : cf. Repas</t>
+    <t xml:space="preserve">code postal de l'adresse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ville où se situe l'adresse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numéro de la rue / avenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rue / avenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nom de la rue / avenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">complementA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">complément d'information sur l'adresse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nomTag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mot permettant d'identifiier une offre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nomRepas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titre du repas servis et Clé primaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{«Petit-déjeuner », « Déjeuner », « Dîner », « Boissons », « Brunch »}</t>
   </si>
   <si>
     <t xml:space="preserve">idAvis</t>
@@ -625,45 +668,6 @@
     <t xml:space="preserve">photo (cf.image)</t>
   </si>
   <si>
-    <t xml:space="preserve">code postal de l'adresse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ville où se situe l'adresse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numéro de la rue / avenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rue / avenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nom de la rue / avenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">complementA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">complément d'information sur l'adresse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idTag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">primary key du tag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nomTag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mot permettant d'identifiier une offre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sous catégorie de tag : cf CaractéristiqueTagAutre, Ca</t>
-  </si>
-  <si>
     <t xml:space="preserve">idImage</t>
   </si>
   <si>
@@ -674,9 +678,6 @@
   </si>
   <si>
     <t xml:space="preserve">url contenant l'image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interval</t>
   </si>
   <si>
     <t xml:space="preserve">serial</t>
@@ -1091,19 +1092,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1845,7 +1846,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1912,7 +1913,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1961,10 +1962,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>34</v>
@@ -1984,10 +1985,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>14</v>
@@ -2007,10 +2008,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>87</v>
@@ -2030,10 +2031,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>34</v>
@@ -2046,17 +2047,17 @@
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>34</v>
@@ -2069,7 +2070,7 @@
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H8" s="23"/>
       <c r="I8" s="19"/>
@@ -2197,7 +2198,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2240,10 +2241,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>34</v>
@@ -2263,10 +2264,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>14</v>
@@ -2279,7 +2280,7 @@
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="19"/>
@@ -2318,10 +2319,371 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:I14"/>
+  <dimension ref="A3:I1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="53.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="36.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="75.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5:C8" type="list">
+      <formula1>Parametres!$A$1:$A$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G5:G8" type="list">
+      <formula1>Parametres!$C$1:$C$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D5:D8" type="list">
+      <formula1>Parametres!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="36.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="75.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D6" type="list">
+      <formula1>Parametres!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4:G6" type="list">
+      <formula1>Parametres!$C$1:$C$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C6" type="list">
+      <formula1>Parametres!$A$1:$A$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:I1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2338,82 +2700,105 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14"/>
+      <c r="A4" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="18"/>
+        <v>141</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="23"/>
       <c r="I5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>122</v>
+        <v>142</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>143</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="22" t="s">
@@ -2423,616 +2808,55 @@
       <c r="I6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="30" t="s">
-        <v>123</v>
+      <c r="A7" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="22" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="19"/>
-    </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="19"/>
+      <c r="A9" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="19"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="19"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="19"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="19"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="19"/>
-    </row>
+      <c r="A10" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5:C14" type="list">
-      <formula1>Parametres!$A$1:$A$9</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G5:G14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D7" type="list">
+      <formula1>Parametres!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4:G7" type="list">
       <formula1>Parametres!$C$1:$C$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D5:D14" type="list">
-      <formula1>Parametres!$B$1:$B$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B2:J13"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="64.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="36.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="75.57"/>
-  </cols>
-  <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="19"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="19"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="19"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="19"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="19"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="19"/>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4:E13" type="list">
-      <formula1>Parametres!$B$1:$B$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H13" type="list">
-      <formula1>Parametres!$C$1:$C$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D13" type="list">
-      <formula1>Parametres!$A$1:$A$9</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B2:J13"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="36.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="75.57"/>
-  </cols>
-  <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="19"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="19"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="19"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="19"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="19"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="19"/>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4:E13" type="list">
-      <formula1>Parametres!$B$1:$B$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H13" type="list">
-      <formula1>Parametres!$C$1:$C$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D13" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C7" type="list">
       <formula1>Parametres!$A$1:$A$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3052,232 +2876,188 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:J13"/>
+  <dimension ref="A2:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="64.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="36.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="75.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="36.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="75.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="9"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="19" t="s">
-        <v>145</v>
+      <c r="F3" s="10"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>148</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>146</v>
+        <v>34</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="29" t="s">
+      <c r="D5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="19"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="F5" s="19"/>
+      <c r="G5" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="26"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="26" t="s">
+      <c r="D7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="19"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="19"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="19"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="19"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="19"/>
-    </row>
+      <c r="F7" s="19"/>
+      <c r="G7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="23"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4:E13" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D7" type="list">
       <formula1>Parametres!$B$1:$B$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H13" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4:G7" type="list">
       <formula1>Parametres!$C$1:$C$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D13" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C5 C7" type="list">
       <formula1>Parametres!$A$1:$A$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3297,238 +3077,137 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:J16"/>
+  <dimension ref="A3:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="36.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="75.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="36.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="33.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" s="15" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="29" t="s">
+      <c r="D5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="19"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" s="21" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="26" t="s">
+      <c r="D6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="19"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="19" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="19" t="s">
+      <c r="F6" s="19"/>
+      <c r="G6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="19"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="19"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="19"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
-        <v>164</v>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4:E13" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5:C6" type="list">
+      <formula1>Parametres!$A$1:$A$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G5:G6" type="list">
+      <formula1>Parametres!$C$1:$C$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D5:D6" type="list">
       <formula1>Parametres!$B$1:$B$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H13" type="list">
-      <formula1>Parametres!$C$1:$C$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D5 D7:D13" type="list">
-      <formula1>Parametres!$A$1:$A$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -3547,214 +3226,147 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:J16"/>
+  <dimension ref="A2:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="33.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="36.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="33.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="36.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="75.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="3"/>
-      <c r="C3" s="4" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="14"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="19" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="19"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="19" t="s">
+      <c r="C5" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="D5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="26" t="s">
         <v>168</v>
       </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>167</v>
+      </c>
       <c r="D6" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="19"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="19"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="19"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="19"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="19"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
+        <v>15</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D5:D14" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D6" type="list">
+      <formula1>Parametres!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4:G6" type="list">
+      <formula1>Parametres!$C$1:$C$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C6" type="list">
       <formula1>Parametres!$A$1:$A$9</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H5:H14" type="list">
-      <formula1>Parametres!$C$1:$C$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E5:E14" type="list">
-      <formula1>Parametres!$B$1:$B$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -3773,23 +3385,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:J18"/>
+  <dimension ref="B2:J8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="47.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="31.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="71.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="39.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.14"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3832,45 +3444,45 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>171</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="26" t="s">
+      <c r="E4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="33" t="s">
         <v>28</v>
       </c>
       <c r="G4" s="19"/>
-      <c r="H4" s="22" t="s">
-        <v>112</v>
+      <c r="H4" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="I4" s="23"/>
       <c r="J4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>173</v>
-      </c>
       <c r="D5" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="34" t="s">
-        <v>88</v>
+        <v>14</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="G5" s="19"/>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="17" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="23"/>
@@ -3878,22 +3490,22 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="19" t="s">
-        <v>106</v>
+        <v>173</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>174</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>28</v>
       </c>
       <c r="G6" s="19"/>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="17" t="s">
         <v>17</v>
       </c>
       <c r="I6" s="23"/>
@@ -3904,201 +3516,58 @@
         <v>175</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G7" s="19"/>
-      <c r="H7" s="22" t="s">
-        <v>112</v>
+      <c r="H7" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="I7" s="23"/>
       <c r="J7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>178</v>
+        <v>14</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="G8" s="19"/>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="17" t="s">
         <v>17</v>
       </c>
       <c r="I8" s="23"/>
       <c r="J8" s="19"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="23"/>
-      <c r="J9" s="19"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="23"/>
-      <c r="J11" s="19"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>185</v>
-      </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="23"/>
-      <c r="J13" s="19"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="19"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="19"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4:E15" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4:E8" type="list">
       <formula1>Parametres!$B$1:$B$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H15" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H8" type="list">
       <formula1>Parametres!$C$1:$C$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D15" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D8" type="list">
       <formula1>Parametres!$A$1:$A$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4252,212 +3721,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:J8"/>
+  <dimension ref="B2:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="39.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.14"/>
-  </cols>
-  <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3"/>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="19"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="19"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="19"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="19"/>
-      <c r="H8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="19"/>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4:E8" type="list">
-      <formula1>Parametres!$B$1:$B$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H8" type="list">
-      <formula1>Parametres!$C$1:$C$2</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D8" type="list">
-      <formula1>Parametres!$A$1:$A$9</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="B2:J11"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4512,17 +3779,17 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="19" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>34</v>
+        <v>180</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="E4" s="21"/>
-      <c r="F4" s="19" t="s">
-        <v>28</v>
+      <c r="F4" s="31" t="s">
+        <v>20</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="22" t="s">
@@ -4531,87 +3798,134 @@
       <c r="I4" s="23"/>
       <c r="J4" s="19"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="19"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="19"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="19"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="19"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4:E9" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4" type="list">
       <formula1>Parametres!$B$1:$B$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H9" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4" type="list">
       <formula1>Parametres!$C$1:$C$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D9" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4" type="list">
+      <formula1>Parametres!$A$1:$A$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:J1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="59.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="51.42"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="23"/>
+      <c r="J4" s="19"/>
+    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4" type="list">
+      <formula1>Parametres!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4" type="list">
+      <formula1>Parametres!$C$1:$C$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4" type="list">
       <formula1>Parametres!$A$1:$A$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4627,6 +3941,351 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:J18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G33" activeCellId="0" sqref="G33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="47.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="31.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="26.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="71.14"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="9"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="14"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" s="23"/>
+      <c r="J4" s="19"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="H5" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="23"/>
+      <c r="J5" s="19"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="19"/>
+      <c r="H6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="23"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="19"/>
+      <c r="H7" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" s="23"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="23"/>
+      <c r="J8" s="19"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="23"/>
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="I10" s="23"/>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="23"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="G12" s="19"/>
+      <c r="H12" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="23"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="23"/>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="19"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4:E15" type="list">
+      <formula1>Parametres!$B$1:$B$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H15" type="list">
+      <formula1>Parametres!$C$1:$C$2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D15" type="list">
+      <formula1>Parametres!$A$1:$A$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4689,10 +4348,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="19" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>34</v>
@@ -4708,10 +4367,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>14</v>
@@ -4794,7 +4453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4829,7 +4488,7 @@
         <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4849,7 +4508,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>209</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4859,7 +4518,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>131</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4878,7 +4537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <tabColor rgb="FFFF4000"/>
@@ -5960,8 +5619,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6196,6 +5855,11 @@
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6300,7 +5964,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>